<commit_message>
keep on cleaning data
</commit_message>
<xml_diff>
--- a/structured_songs_data.xlsx
+++ b/structured_songs_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rainylty/STUDY/IVth/datascience/summer_school/summoning_and_lotr/Viz_of_Summoning_and_Middle_Earth-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7852E604-2A6F-9B47-9962-A746B24C91DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07E6220-E52B-574A-9930-7F016846D076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4400" yWindow="500" windowWidth="25280" windowHeight="21900" xr2:uid="{5E9570CC-4598-2A4D-A4CD-D4496BCFE1CA}"/>
+    <workbookView xWindow="3720" yWindow="500" windowWidth="26720" windowHeight="21900" xr2:uid="{5E9570CC-4598-2A4D-A4CD-D4496BCFE1CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="181">
   <si>
     <t>Lugburz</t>
   </si>
@@ -542,6 +542,45 @@
   </si>
   <si>
     <t>In Khazad-dûm his wisdom died</t>
+  </si>
+  <si>
+    <t>At the stone of Erech they shall stand again</t>
+  </si>
+  <si>
+    <t>To the Paths of the Dead</t>
+  </si>
+  <si>
+    <t>Paths of the Dead</t>
+  </si>
+  <si>
+    <t>Kôrtirion</t>
+  </si>
+  <si>
+    <t>The Cottage of Lost Play</t>
+  </si>
+  <si>
+    <t>https://lotr.fandom.com/wiki/Cottage_of_Lost_Play</t>
+  </si>
+  <si>
+    <t>Tol Eressëa</t>
+  </si>
+  <si>
+    <t>The Lonely Island, The Lonely Isle, Eressëa</t>
+  </si>
+  <si>
+    <t>island</t>
+  </si>
+  <si>
+    <t>Off the east coast of Aman in the Bay of Eldamar</t>
+  </si>
+  <si>
+    <t>Rhûn</t>
+  </si>
+  <si>
+    <t>The East, Eastlands</t>
+  </si>
+  <si>
+    <t>All thy trees, Kôrtirion, were bent, since first the elves here built ancient, renowned Kôrtirion</t>
   </si>
 </sst>
 </file>
@@ -572,7 +611,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -597,12 +636,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -617,7 +650,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -627,7 +660,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -943,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0522EB-0476-FB45-AC71-51653D98331B}">
-  <dimension ref="A1:N77"/>
+  <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1715,15 +1747,21 @@
       <c r="I35" s="6"/>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="7">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36">
         <v>1997</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" t="s">
         <v>24</v>
+      </c>
+      <c r="D36" t="s">
+        <v>180</v>
+      </c>
+      <c r="E36" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
@@ -1736,38 +1774,68 @@
       <c r="C37" t="s">
         <v>25</v>
       </c>
+      <c r="D37" t="s">
+        <v>168</v>
+      </c>
+      <c r="E37" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="B38" t="s">
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D38" t="s">
+        <v>169</v>
+      </c>
+      <c r="E38" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="D39" t="s">
+        <v>172</v>
+      </c>
+      <c r="E39" t="s">
+        <v>174</v>
+      </c>
+      <c r="F39" t="s">
+        <v>175</v>
+      </c>
+      <c r="H39" t="s">
+        <v>176</v>
+      </c>
+      <c r="J39" t="s">
+        <v>177</v>
+      </c>
+      <c r="N39" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>1999</v>
-      </c>
-      <c r="B40" t="s">
-        <v>3</v>
-      </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>178</v>
+      </c>
+      <c r="D40" t="s">
+        <v>178</v>
+      </c>
+      <c r="F40" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
@@ -1778,7 +1846,7 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
@@ -1789,7 +1857,7 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
@@ -1800,7 +1868,7 @@
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
@@ -1811,7 +1879,7 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
@@ -1822,7 +1890,7 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
@@ -1833,29 +1901,29 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1866,7 +1934,7 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1877,7 +1945,7 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1888,7 +1956,7 @@
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1899,7 +1967,7 @@
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1910,7 +1978,7 @@
         <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1921,29 +1989,29 @@
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>2006</v>
+        <v>2001</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>2006</v>
+        <v>2001</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1954,7 +2022,7 @@
         <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1965,7 +2033,7 @@
         <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1976,7 +2044,7 @@
         <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1987,7 +2055,7 @@
         <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1998,7 +2066,7 @@
         <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -2009,29 +2077,29 @@
         <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="B64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -2042,7 +2110,7 @@
         <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -2053,7 +2121,7 @@
         <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -2064,7 +2132,7 @@
         <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -2075,7 +2143,7 @@
         <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -2086,7 +2154,7 @@
         <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -2097,29 +2165,29 @@
         <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C71" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -2130,7 +2198,7 @@
         <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -2141,7 +2209,7 @@
         <v>7</v>
       </c>
       <c r="C74" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -2152,7 +2220,7 @@
         <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -2163,7 +2231,7 @@
         <v>7</v>
       </c>
       <c r="C76" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -2174,6 +2242,28 @@
         <v>7</v>
       </c>
       <c r="C77" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>2018</v>
+      </c>
+      <c r="B78" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>2018</v>
+      </c>
+      <c r="B79" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correct mistakes in geodata cleaning
</commit_message>
<xml_diff>
--- a/structured_songs_data.xlsx
+++ b/structured_songs_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rainylty/STUDY/IVth/datascience/summer_school/summoning_and_lotr/Viz_of_Summoning_and_Middle_Earth-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E391966-352D-6747-AC14-CD98910F2CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A18379-81A3-0348-84CD-4242574B5D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12000" yWindow="500" windowWidth="18400" windowHeight="21900" xr2:uid="{5E9570CC-4598-2A4D-A4CD-D4496BCFE1CA}"/>
+    <workbookView xWindow="7800" yWindow="500" windowWidth="18400" windowHeight="21900" xr2:uid="{5E9570CC-4598-2A4D-A4CD-D4496BCFE1CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="227">
   <si>
     <t>Lugburz</t>
   </si>
@@ -713,13 +713,19 @@
   </si>
   <si>
     <t>https://lotr.fandom.com/wiki/Herumor</t>
+  </si>
+  <si>
+    <t>Númenor(Black Númenóreans)</t>
+  </si>
+  <si>
+    <t>In later days when Morgoth first</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -738,6 +744,14 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -788,7 +802,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -799,6 +813,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1114,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0522EB-0476-FB45-AC71-51653D98331B}">
-  <dimension ref="A1:O80"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J61" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q94" sqref="Q94"/>
+    <sheetView tabSelected="1" topLeftCell="D89" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2361,7 +2377,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2006</v>
       </c>
@@ -2381,7 +2397,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2013</v>
       </c>
@@ -2392,7 +2408,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2013</v>
       </c>
@@ -2418,7 +2434,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2013</v>
       </c>
@@ -2429,7 +2445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2013</v>
       </c>
@@ -2464,7 +2480,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2013</v>
       </c>
@@ -2490,7 +2506,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2013</v>
       </c>
@@ -2501,7 +2517,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2013</v>
       </c>
@@ -2512,7 +2528,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2013</v>
       </c>
@@ -2523,7 +2539,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2018</v>
       </c>
@@ -2552,7 +2568,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2018</v>
       </c>
@@ -2581,7 +2597,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2018</v>
       </c>
@@ -2601,7 +2617,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2018</v>
       </c>
@@ -2611,11 +2627,20 @@
       <c r="C77" t="s">
         <v>61</v>
       </c>
+      <c r="D77" t="s">
+        <v>225</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="I77" t="s">
+        <v>218</v>
+      </c>
       <c r="N77" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2018</v>
       </c>
@@ -2626,7 +2651,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2018</v>
       </c>
@@ -2637,7 +2662,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2018</v>
       </c>
@@ -2647,6 +2672,31 @@
       <c r="C80" t="s">
         <v>64</v>
       </c>
+      <c r="D80" t="s">
+        <v>226</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="I80" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="J80" s="8"/>
+      <c r="K80" s="8"/>
+      <c r="L80" s="8"/>
+      <c r="M80" s="8"/>
+      <c r="N80" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="O80" s="9"/>
+      <c r="P80" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2661,6 +2711,7 @@
     <hyperlink ref="N74" r:id="rId9" xr:uid="{E519F547-03AC-FA4A-8730-D014042DF8CB}"/>
     <hyperlink ref="O74" r:id="rId10" xr:uid="{7E05CD30-8908-B545-B3A2-FDBAF51DDF43}"/>
     <hyperlink ref="N77" r:id="rId11" xr:uid="{0B521D66-5ABC-2C45-93FA-2CD73EF8875A}"/>
+    <hyperlink ref="N80" r:id="rId12" xr:uid="{B76E97F0-956E-DC4D-9392-C2E9200A4A57}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>